<commit_message>
Change the class impl.util.XlsWriter:
Delete fields: currentRow, titleRow, titleCell,
cellStyle, alignment.
Add fields: arrayCellStyles, arrayFonts, row, cell.
Add methods: setFont(), setStyle, fillRow.
Add interface ValueOfStatistics.
Add nested static classes: StringValue, IntValue,
FloatValue.
</commit_message>
<xml_diff>
--- a/src/main/resources/test.xlsx
+++ b/src/main/resources/test.xlsx
@@ -55,13 +55,22 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -84,8 +93,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyAlignment="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
@@ -105,16 +120,16 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="1">
         <v>3</v>
       </c>
     </row>
@@ -122,13 +137,13 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" t="n" s="2">
         <v>4.550000190734863</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" t="n" s="2">
         <v>2.0</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2" t="n" s="2">
         <v>2.0</v>
       </c>
     </row>
@@ -136,13 +151,13 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" t="n" s="2">
         <v>3.799999952316284</v>
       </c>
-      <c r="C3" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D3" t="n">
+      <c r="C3" t="n" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D3" t="n" s="2">
         <v>1.0</v>
       </c>
     </row>
@@ -150,13 +165,13 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" t="n" s="2">
         <v>3.5</v>
       </c>
-      <c r="C4" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D4" t="n">
+      <c r="C4" t="n" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D4" t="n" s="2">
         <v>1.0</v>
       </c>
     </row>
@@ -164,13 +179,13 @@
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" t="n" s="2">
         <v>4.300000190734863</v>
       </c>
-      <c r="C5" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D5" t="n">
+      <c r="C5" t="n" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D5" t="n" s="2">
         <v>1.0</v>
       </c>
     </row>
@@ -178,13 +193,13 @@
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" t="n" s="2">
         <v>4.900000095367432</v>
       </c>
-      <c r="C6" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D6" t="n">
+      <c r="C6" t="n" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D6" t="n" s="2">
         <v>1.0</v>
       </c>
     </row>
@@ -192,13 +207,13 @@
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" t="n" s="2">
         <v>5.0</v>
       </c>
-      <c r="C7" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D7" t="n">
+      <c r="C7" t="n" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D7" t="n" s="2">
         <v>1.0</v>
       </c>
     </row>
@@ -206,13 +221,13 @@
       <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8" t="n" s="2">
         <v>4.0</v>
       </c>
-      <c r="C8" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D8" t="n">
+      <c r="C8" t="n" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="D8" t="n" s="2">
         <v>1.0</v>
       </c>
     </row>
@@ -220,13 +235,13 @@
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9" t="n" s="2">
         <v>0.0</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9" t="n" s="2">
         <v>0.0</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9" t="n" s="2">
         <v>1.0</v>
       </c>
     </row>

</xml_diff>